<commit_message>
Updated to include Median Income, SNAP
</commit_message>
<xml_diff>
--- a/madisonData.xlsx
+++ b/madisonData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chock\Desktop\school\GRAD\OM516\dev\OMP1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB14F615-38D0-41AA-8CA3-83A0E96FD9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1968E60A-EA99-4222-BB7E-CDF3041C9010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="0" windowWidth="13147" windowHeight="8460" xr2:uid="{117D388F-8E02-48E4-BAB9-6DBDE62B405D}"/>
+    <workbookView xWindow="11168" yWindow="0" windowWidth="11415" windowHeight="14362" xr2:uid="{117D388F-8E02-48E4-BAB9-6DBDE62B405D}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Year</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>Consumer Price Index</t>
+  </si>
+  <si>
+    <t>Median Household Income</t>
+  </si>
+  <si>
+    <t>SNAP Recipients</t>
   </si>
 </sst>
 </file>
@@ -66,7 +72,7 @@
   <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="168" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -110,7 +116,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71998E2C-729F-4B9C-B948-8EA96E1EC4B2}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -460,9 +466,11 @@
     <col min="5" max="5" width="12.3984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -484,8 +492,14 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>2022</v>
       </c>
@@ -507,8 +521,14 @@
       <c r="G2" s="4">
         <v>292.65499999999997</v>
       </c>
+      <c r="H2">
+        <v>80426</v>
+      </c>
+      <c r="I2">
+        <v>36551</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2021</v>
       </c>
@@ -530,8 +550,14 @@
       <c r="G3" s="4">
         <v>270.97000000000003</v>
       </c>
+      <c r="H3">
+        <v>78386</v>
+      </c>
+      <c r="I3">
+        <v>37964</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -553,8 +579,14 @@
       <c r="G4" s="4">
         <v>258.81099999999998</v>
       </c>
+      <c r="H4">
+        <v>67810</v>
+      </c>
+      <c r="I4">
+        <v>37893</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>2019</v>
       </c>
@@ -576,8 +608,14 @@
       <c r="G5" s="4">
         <v>255.65700000000001</v>
       </c>
+      <c r="H5">
+        <v>68609</v>
+      </c>
+      <c r="I5">
+        <v>36578</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>2018</v>
       </c>
@@ -599,8 +637,14 @@
       <c r="G6" s="4">
         <v>251.107</v>
       </c>
+      <c r="H6">
+        <v>63755</v>
+      </c>
+      <c r="I6">
+        <v>37088</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>2017</v>
       </c>
@@ -621,6 +665,12 @@
       </c>
       <c r="G7" s="4">
         <v>245.12</v>
+      </c>
+      <c r="H7">
+        <v>62750</v>
+      </c>
+      <c r="I7">
+        <v>38675</v>
       </c>
     </row>
   </sheetData>

</xml_diff>